<commit_message>
hot fix embarrada Pablo :(
</commit_message>
<xml_diff>
--- a/data base/onAirCampos.xlsx
+++ b/data base/onAirCampos.xlsx
@@ -3137,12 +3137,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:L147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3389,7 +3388,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="6" customFormat="1" hidden="1">
+    <row r="9" spans="1:11" s="6" customFormat="1">
       <c r="A9" s="6" t="s">
         <v>142</v>
       </c>
@@ -3421,7 +3420,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="6" customFormat="1" hidden="1">
+    <row r="10" spans="1:11" s="6" customFormat="1">
       <c r="A10" s="6" t="s">
         <v>143</v>
       </c>
@@ -3537,7 +3536,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="6" customFormat="1" hidden="1">
+    <row r="14" spans="1:11" s="6" customFormat="1">
       <c r="A14" s="6" t="s">
         <v>147</v>
       </c>
@@ -3833,7 +3832,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="6" customFormat="1" hidden="1">
+    <row r="24" spans="1:11" s="6" customFormat="1">
       <c r="A24" s="6" t="s">
         <v>157</v>
       </c>
@@ -3952,7 +3951,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="6" customFormat="1" hidden="1">
+    <row r="28" spans="1:11" s="6" customFormat="1">
       <c r="A28" s="6" t="s">
         <v>161</v>
       </c>
@@ -3984,7 +3983,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="6" customFormat="1" hidden="1">
+    <row r="29" spans="1:11" s="6" customFormat="1">
       <c r="A29" s="6" t="s">
         <v>162</v>
       </c>
@@ -4016,7 +4015,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="6" customFormat="1" hidden="1">
+    <row r="30" spans="1:11" s="6" customFormat="1">
       <c r="A30" s="6" t="s">
         <v>163</v>
       </c>
@@ -4045,7 +4044,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="6" customFormat="1" hidden="1">
+    <row r="31" spans="1:11" s="6" customFormat="1">
       <c r="A31" s="6" t="s">
         <v>164</v>
       </c>
@@ -4100,7 +4099,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="6" customFormat="1" hidden="1">
+    <row r="33" spans="1:11" s="6" customFormat="1">
       <c r="A33" s="6" t="s">
         <v>166</v>
       </c>
@@ -4129,7 +4128,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="6" customFormat="1" hidden="1">
+    <row r="34" spans="1:11" s="6" customFormat="1">
       <c r="A34" s="6" t="s">
         <v>167</v>
       </c>
@@ -4158,7 +4157,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="6" customFormat="1" hidden="1">
+    <row r="35" spans="1:11" s="6" customFormat="1">
       <c r="A35" s="6" t="s">
         <v>168</v>
       </c>
@@ -4280,7 +4279,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="39" spans="1:11" s="6" customFormat="1" hidden="1">
+    <row r="39" spans="1:11" s="6" customFormat="1">
       <c r="A39" s="6" t="s">
         <v>172</v>
       </c>
@@ -4312,7 +4311,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="40" spans="1:11" s="6" customFormat="1" hidden="1">
+    <row r="40" spans="1:11" s="6" customFormat="1">
       <c r="A40" s="6" t="s">
         <v>173</v>
       </c>
@@ -4570,7 +4569,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="6" customFormat="1" hidden="1">
+    <row r="49" spans="1:12" s="6" customFormat="1">
       <c r="A49" s="6" t="s">
         <v>182</v>
       </c>
@@ -4599,7 +4598,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="50" spans="1:12" s="6" customFormat="1" hidden="1">
+    <row r="50" spans="1:12" s="6" customFormat="1">
       <c r="A50" s="6" t="s">
         <v>183</v>
       </c>
@@ -4628,7 +4627,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="51" spans="1:12" s="6" customFormat="1" hidden="1">
+    <row r="51" spans="1:12" s="6" customFormat="1">
       <c r="A51" s="6" t="s">
         <v>184</v>
       </c>
@@ -4657,7 +4656,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="52" spans="1:12" s="6" customFormat="1" hidden="1">
+    <row r="52" spans="1:12" s="6" customFormat="1">
       <c r="A52" s="6" t="s">
         <v>185</v>
       </c>
@@ -4749,7 +4748,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="56" spans="1:12" s="6" customFormat="1" hidden="1">
+    <row r="56" spans="1:12" s="6" customFormat="1">
       <c r="A56" s="6" t="s">
         <v>189</v>
       </c>
@@ -4775,7 +4774,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="57" spans="1:12" s="6" customFormat="1" hidden="1">
+    <row r="57" spans="1:12" s="6" customFormat="1">
       <c r="A57" s="6" t="s">
         <v>190</v>
       </c>
@@ -4801,7 +4800,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="58" spans="1:12" s="1" customFormat="1" hidden="1">
+    <row r="58" spans="1:12" s="1" customFormat="1">
       <c r="A58" s="1" t="s">
         <v>191</v>
       </c>
@@ -4833,7 +4832,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="59" spans="1:12" s="1" customFormat="1" hidden="1">
+    <row r="59" spans="1:12" s="1" customFormat="1">
       <c r="A59" s="1" t="s">
         <v>192</v>
       </c>
@@ -4865,7 +4864,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="60" spans="1:12" s="1" customFormat="1" hidden="1">
+    <row r="60" spans="1:12" s="1" customFormat="1">
       <c r="A60" s="1" t="s">
         <v>193</v>
       </c>
@@ -4891,7 +4890,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="61" spans="1:12" s="1" customFormat="1" hidden="1">
+    <row r="61" spans="1:12" s="1" customFormat="1">
       <c r="A61" s="1" t="s">
         <v>194</v>
       </c>
@@ -4917,7 +4916,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="62" spans="1:12" s="1" customFormat="1" hidden="1">
+    <row r="62" spans="1:12" s="1" customFormat="1">
       <c r="A62" s="1" t="s">
         <v>195</v>
       </c>
@@ -4940,7 +4939,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="63" spans="1:12" s="1" customFormat="1" hidden="1">
+    <row r="63" spans="1:12" s="1" customFormat="1">
       <c r="A63" s="1" t="s">
         <v>196</v>
       </c>
@@ -4966,7 +4965,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="64" spans="1:12" s="1" customFormat="1" hidden="1">
+    <row r="64" spans="1:12" s="1" customFormat="1">
       <c r="A64" s="1" t="s">
         <v>197</v>
       </c>
@@ -4989,7 +4988,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="65" spans="1:12" s="1" customFormat="1" hidden="1">
+    <row r="65" spans="1:12" s="1" customFormat="1">
       <c r="A65" s="1" t="s">
         <v>198</v>
       </c>
@@ -5015,7 +5014,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="66" spans="1:12" s="1" customFormat="1" hidden="1">
+    <row r="66" spans="1:12" s="1" customFormat="1">
       <c r="A66" s="1" t="s">
         <v>199</v>
       </c>
@@ -5038,7 +5037,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="67" spans="1:12" s="1" customFormat="1" hidden="1">
+    <row r="67" spans="1:12" s="1" customFormat="1">
       <c r="A67" s="1" t="s">
         <v>200</v>
       </c>
@@ -5064,7 +5063,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="68" spans="1:12" s="1" customFormat="1" hidden="1">
+    <row r="68" spans="1:12" s="1" customFormat="1">
       <c r="A68" s="1" t="s">
         <v>201</v>
       </c>
@@ -5087,7 +5086,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="69" spans="1:12" s="1" customFormat="1" hidden="1">
+    <row r="69" spans="1:12" s="1" customFormat="1">
       <c r="A69" s="1" t="s">
         <v>202</v>
       </c>
@@ -5113,7 +5112,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="70" spans="1:12" s="1" customFormat="1" hidden="1">
+    <row r="70" spans="1:12" s="1" customFormat="1">
       <c r="A70" s="1" t="s">
         <v>203</v>
       </c>
@@ -5136,7 +5135,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="71" spans="1:12" s="1" customFormat="1" hidden="1">
+    <row r="71" spans="1:12" s="1" customFormat="1">
       <c r="A71" s="1" t="s">
         <v>204</v>
       </c>
@@ -5162,7 +5161,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="72" spans="1:12" s="1" customFormat="1" hidden="1">
+    <row r="72" spans="1:12" s="1" customFormat="1">
       <c r="A72" s="1" t="s">
         <v>205</v>
       </c>
@@ -5185,7 +5184,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="73" spans="1:12" s="1" customFormat="1" hidden="1">
+    <row r="73" spans="1:12" s="1" customFormat="1">
       <c r="A73" s="1" t="s">
         <v>206</v>
       </c>
@@ -5271,7 +5270,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="77" spans="1:12" s="6" customFormat="1" hidden="1">
+    <row r="77" spans="1:12" s="6" customFormat="1">
       <c r="A77" s="6" t="s">
         <v>210</v>
       </c>
@@ -5300,7 +5299,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="78" spans="1:12" s="6" customFormat="1" hidden="1">
+    <row r="78" spans="1:12" s="6" customFormat="1">
       <c r="A78" s="6" t="s">
         <v>211</v>
       </c>
@@ -5393,7 +5392,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="81" spans="1:12" s="6" customFormat="1" hidden="1">
+    <row r="81" spans="1:12" s="6" customFormat="1">
       <c r="A81" s="6" t="s">
         <v>214</v>
       </c>
@@ -5422,7 +5421,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="82" spans="1:12" s="6" customFormat="1" hidden="1">
+    <row r="82" spans="1:12" s="6" customFormat="1">
       <c r="A82" s="6" t="s">
         <v>215</v>
       </c>
@@ -5924,7 +5923,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="99" spans="1:10" s="6" customFormat="1" hidden="1">
+    <row r="99" spans="1:10" s="6" customFormat="1">
       <c r="A99" s="6" t="s">
         <v>232</v>
       </c>
@@ -5953,7 +5952,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="100" spans="1:10" s="6" customFormat="1" hidden="1">
+    <row r="100" spans="1:10" s="6" customFormat="1">
       <c r="A100" s="6" t="s">
         <v>233</v>
       </c>
@@ -5979,7 +5978,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="101" spans="1:10" s="6" customFormat="1" hidden="1">
+    <row r="101" spans="1:10" s="6" customFormat="1">
       <c r="A101" s="6" t="s">
         <v>234</v>
       </c>
@@ -6027,7 +6026,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="104" spans="1:10" s="6" customFormat="1" hidden="1">
+    <row r="104" spans="1:10" s="6" customFormat="1">
       <c r="A104" s="6" t="s">
         <v>237</v>
       </c>
@@ -6108,7 +6107,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="107" spans="1:10" s="6" customFormat="1" hidden="1">
+    <row r="107" spans="1:10" s="6" customFormat="1">
       <c r="A107" s="6" t="s">
         <v>240</v>
       </c>
@@ -6137,7 +6136,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="108" spans="1:10" s="6" customFormat="1" hidden="1">
+    <row r="108" spans="1:10" s="6" customFormat="1">
       <c r="A108" s="6" t="s">
         <v>241</v>
       </c>
@@ -6166,7 +6165,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="109" spans="1:10" s="6" customFormat="1" hidden="1">
+    <row r="109" spans="1:10" s="6" customFormat="1">
       <c r="A109" s="6" t="s">
         <v>243</v>
       </c>
@@ -6195,7 +6194,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="110" spans="1:10" s="6" customFormat="1" hidden="1">
+    <row r="110" spans="1:10" s="6" customFormat="1">
       <c r="A110" s="6" t="s">
         <v>244</v>
       </c>
@@ -6224,7 +6223,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="111" spans="1:10" s="6" customFormat="1" hidden="1">
+    <row r="111" spans="1:10" s="6" customFormat="1">
       <c r="A111" s="6" t="s">
         <v>245</v>
       </c>
@@ -6473,7 +6472,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="120" spans="1:11" s="6" customFormat="1" hidden="1">
+    <row r="120" spans="1:11" s="6" customFormat="1">
       <c r="A120" s="6" t="s">
         <v>254</v>
       </c>
@@ -6975,29 +6974,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I147">
-    <filterColumn colId="3">
-      <filters blank="1">
-        <filter val="Ing"/>
-        <filter val="sistema"/>
-        <filter val="sitema"/>
-        <filter val="usuario"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters blank="1">
-        <filter val="inicio"/>
-        <filter val="inicio*"/>
-        <filter val="inicio,todas"/>
-        <filter val="precheck"/>
-        <filter val="preck"/>
-        <filter val="seguimiento 12H"/>
-        <filter val="seguimiento 24H"/>
-        <filter val="seguimiento 36H"/>
-        <filter val="seguimiento 48H"/>
-        <filter val="seguimiento 4H, seguimiento 8H, seguimiento 12H;seguimiento 24H, seguimiento 36H"/>
-        <filter val="todas"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="3"/>
+    <filterColumn colId="5"/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>